<commit_message>
Updated version of MultiYear
Time_Series.xlsx prints each year in a different sheet;
The litres of fuel consumed are printed in Time_Series.xlsx;
</commit_message>
<xml_diff>
--- a/MicroGrids/Results/Generator_Data.xlsx
+++ b/MicroGrids/Results/Generator_Data.xlsx
@@ -449,7 +449,7 @@
         <v>5</v>
       </c>
       <c r="B6">
-        <v>16176.90177302888</v>
+        <v>16477.85834047381</v>
       </c>
     </row>
     <row r="7" spans="1:2">
@@ -465,7 +465,7 @@
         <v>7</v>
       </c>
       <c r="B8">
-        <v>23941.81462408275</v>
+        <v>24387.23034390124</v>
       </c>
     </row>
     <row r="9" spans="1:2">
@@ -473,7 +473,7 @@
         <v>8</v>
       </c>
       <c r="B9">
-        <v>1077.381658083724</v>
+        <v>1097.425365475556</v>
       </c>
     </row>
     <row r="10" spans="1:2">

</xml_diff>